<commit_message>
Update description field in archival enhanced templates
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/archival-mods-template-enhanced.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/archival-mods-template-enhanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01786FAD-E7ED-4DED-AA71-07132939558E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE22F2C-3CE1-4534-8938-78DB96D7D72B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="555" windowWidth="25845" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="420" windowWidth="28125" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Collection Number</t>
   </si>
   <si>
-    <t>&lt;mods:note displayLabel="Description" type="local"&gt;</t>
-  </si>
-  <si>
     <t>Description of folder contents</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>&lt;/mods:mods&gt;&lt;/datastream&gt;&lt;/object&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mods:note displayLabel="Description"&gt;</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -581,16 +581,16 @@
         <v>8</v>
       </c>
       <c r="V2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="Y2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -602,18 +602,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,18 +834,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2218DF2E-8B03-41C5-82BD-4E07ED3AC316}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48E12C0E-954A-4EBF-8B0C-CA38C7369109}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2218DF2E-8B03-41C5-82BD-4E07ED3AC316}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix whitespace error in description field
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/ExceltoMODSWF/archival-mods-template-enhanced.xlsx
+++ b/DCR_MODS_templates/ExceltoMODSWF/archival-mods-template-enhanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE22F2C-3CE1-4534-8938-78DB96D7D72B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5776E90D-089C-4ECC-B6D8-489FE96876EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="420" windowWidth="28125" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="1425" windowWidth="25980" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <t>&lt;/mods:mods&gt;&lt;/datastream&gt;&lt;/object&gt;</t>
   </si>
   <si>
-    <t>&lt;mods:note displayLabel="Description"&gt;</t>
+    <t>&lt;mods:note displayLabel="Description"&gt;</t>
   </si>
 </sst>
 </file>
@@ -602,21 +602,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100060CAEA771823F4F9BA21EE45585473F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c823f7b768b656f654f262873a6854f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81007de4-ee29-48be-8634-4fbb6dd6f763" xmlns:ns3="fdb5634d-e10a-4de6-afed-2492c365d474" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd052af535147c2bf9c2ace5143a7237" ns2:_="" ns3:_="">
     <xsd:import namespace="81007de4-ee29-48be-8634-4fbb6dd6f763"/>
@@ -833,24 +818,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2218DF2E-8B03-41C5-82BD-4E07ED3AC316}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48E12C0E-954A-4EBF-8B0C-CA38C7369109}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C1DB513-A53A-428B-AA1B-CA693350680F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -867,4 +850,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48E12C0E-954A-4EBF-8B0C-CA38C7369109}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2218DF2E-8B03-41C5-82BD-4E07ED3AC316}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>